<commit_message>
visualization improvement in graphics
</commit_message>
<xml_diff>
--- a/Bench-in-loop/Dense_Linear_Algebra/DLA comparison.xlsx
+++ b/Bench-in-loop/Dense_Linear_Algebra/DLA comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ikerlan-my.sharepoint.com/personal/mrodriguez_ikerlan_es/Documents/Documentos/GitHub/MARS-data/Bench-in-loop/Dense_Linear_Algebra/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="398" documentId="8_{D0BF2C62-6C53-42BC-8F11-EACCC5E617D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{822B3585-4723-41C2-AB58-BC3ABAA9D768}"/>
+  <xr:revisionPtr revIDLastSave="473" documentId="8_{D0BF2C62-6C53-42BC-8F11-EACCC5E617D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17E6B001-14F4-444E-A404-597A1B17199A}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="748" activeTab="2" xr2:uid="{3BB41F9D-0BB3-4FC4-952D-A48197C80458}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="748" activeTab="4" xr2:uid="{3BB41F9D-0BB3-4FC4-952D-A48197C80458}"/>
   </bookViews>
   <sheets>
     <sheet name="gaussian3" sheetId="19" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Kmeans819200" sheetId="23" r:id="rId6"/>
     <sheet name="Streamcluster" sheetId="15" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -487,7 +487,7 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:view3D>
-      <c:rotX val="40"/>
+      <c:rotX val="50"/>
       <c:rotY val="20"/>
       <c:rAngAx val="0"/>
       <c:perspective val="0"/>
@@ -531,9 +531,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.7206391626089008E-2"/>
+          <c:x val="0.14416068266684748"/>
           <c:y val="2.2770647303387497E-2"/>
-          <c:w val="0.74041050325388946"/>
+          <c:w val="0.62689420344822466"/>
           <c:h val="0.81955410382548477"/>
         </c:manualLayout>
       </c:layout>
@@ -542,8 +542,133 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="4"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>TOTAL EXEC</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>(gaussian3!$A$1,gaussian3!$A$11,gaussian3!$A$21,gaussian3!$A$31,gaussian3!$A$41)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>traditional Allocation</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OPT traditional Allocation</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ScatterAlloc</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Zero-Copy</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Unified Memory</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(gaussian3!$K$9,gaussian3!$K$19,gaussian3!$K$29,gaussian3!$K$39,gaussian3!$K$49)</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.94730863619975569</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0951631007176339</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9341924124389076</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0806392775747995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-4090-4208-93DC-0834A68FB2CB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="1"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>COPY API</c:v>
           </c:tx>
@@ -663,130 +788,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-5A59-4191-B28B-1F90070C00D9}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>TOTAL EXEC</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-            <a:sp3d/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="bg1"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="es-ES"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>(gaussian3!$A$1,gaussian3!$A$11,gaussian3!$A$21,gaussian3!$A$31,gaussian3!$A$41)</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>traditional Allocation</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>OPT traditional Allocation</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>ScatterAlloc</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Zero-Copy</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Unified Memory</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>(gaussian3!$K$9,gaussian3!$K$19,gaussian3!$K$29,gaussian3!$K$39,gaussian3!$K$49)</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.94730863619975569</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0951631007176339</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.9341924124389076</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.0806392775747995</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-4090-4208-93DC-0834A68FB2CB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -933,6 +934,27 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.70339571733881E-3"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-D93D-4694-8587-12C191275F5C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
@@ -1058,6 +1080,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1482,9 +1505,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.7206391626089008E-2"/>
+          <c:x val="0.10872818166412472"/>
           <c:y val="2.2770647303387497E-2"/>
-          <c:w val="0.74041050325388946"/>
+          <c:w val="0.64074055244873751"/>
           <c:h val="0.81955410382548477"/>
         </c:manualLayout>
       </c:layout>
@@ -1651,6 +1674,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -2135,8 +2159,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="5.3354129750327751E-2"/>
-              <c:y val="0.28005415156748054"/>
+              <c:x val="2.4658391233124324E-2"/>
+              <c:y val="0.4275103792836536"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2341,9 +2365,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.7206391626089008E-2"/>
+          <c:x val="0.11722815342032425"/>
           <c:y val="2.2770647303387497E-2"/>
-          <c:w val="0.74041050325388946"/>
+          <c:w val="0.65388832401287922"/>
           <c:h val="0.81955410382548477"/>
         </c:manualLayout>
       </c:layout>
@@ -2494,6 +2518,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -2962,8 +2987,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="2.9554040693136285E-2"/>
-              <c:y val="0.3104039574392527"/>
+              <c:x val="2.0586623736089934E-2"/>
+              <c:y val="0.39091550244466811"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -3168,9 +3193,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.7206391626089008E-2"/>
+          <c:x val="9.0155482121674291E-2"/>
           <c:y val="2.2770647303387497E-2"/>
-          <c:w val="0.74041050325388946"/>
+          <c:w val="0.6425340337795854"/>
           <c:h val="0.81955410382548477"/>
         </c:manualLayout>
       </c:layout>
@@ -3337,6 +3362,27 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.7934813308478788E-3"/>
+                  <c:y val="1.3432117568046409E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-9638-4B4A-AF37-634322EBBE2B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
@@ -3470,6 +3516,27 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-1.3432117568046367E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-9638-4B4A-AF37-634322EBBE2B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
@@ -3822,8 +3889,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="2.9396031213587095E-2"/>
-              <c:y val="0.30533599067735151"/>
+              <c:x val="2.0428599672371917E-2"/>
+              <c:y val="0.37473527975645915"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -6012,9 +6079,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.7206391626089008E-2"/>
+          <c:x val="0.10797410570447549"/>
           <c:y val="2.2770647303387497E-2"/>
-          <c:w val="0.74041050325388946"/>
+          <c:w val="0.6462129099060212"/>
           <c:h val="0.81955410382548477"/>
         </c:manualLayout>
       </c:layout>
@@ -6181,6 +6248,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -6288,8 +6356,141 @@
           </c:extLst>
         </c:ser>
         <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>gaussian3!$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>kernels: Fan2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>(gaussian3!$A$1,gaussian3!$A$11,gaussian3!$A$21,gaussian3!$A$31,gaussian3!$A$41)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>traditional Allocation</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OPT traditional Allocation</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ScatterAlloc</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Zero-Copy</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Unified Memory</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(gaussian3!$J$9,gaussian3!$J$19,gaussian3!$J$29,gaussian3!$J$39,gaussian3!$J$49)</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0615478549110928</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0145435080720997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0148200229058613</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1138172721264739</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5A59-4191-B28B-1F90070C00D9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="3"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>gaussian3!$I$4</c:f>
@@ -6417,139 +6618,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-5A59-4191-B28B-1F90070C00D9}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>gaussian3!$J$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>kernels: Fan2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-            <a:sp3d/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="bg1"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="es-ES"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>(gaussian3!$A$1,gaussian3!$A$11,gaussian3!$A$21,gaussian3!$A$31,gaussian3!$A$41)</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>traditional Allocation</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>OPT traditional Allocation</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>ScatterAlloc</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Zero-Copy</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Unified Memory</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>(gaussian3!$J$9,gaussian3!$J$19,gaussian3!$J$29,gaussian3!$J$39,gaussian3!$J$49)</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0615478549110928</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0145435080720997</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.0148200229058613</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.1138172721264739</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5A59-4191-B28B-1F90070C00D9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8245,7 +8313,7 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:view3D>
-      <c:rotX val="40"/>
+      <c:rotX val="50"/>
       <c:rotY val="20"/>
       <c:rAngAx val="0"/>
       <c:perspective val="0"/>
@@ -8289,10 +8357,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.7206391626089008E-2"/>
+          <c:x val="0.11155721262495026"/>
           <c:y val="2.2770647303387497E-2"/>
-          <c:w val="0.74041050325388946"/>
-          <c:h val="0.81955410382548477"/>
+          <c:w val="0.65980529904836061"/>
+          <c:h val="0.82849078178875524"/>
         </c:manualLayout>
       </c:layout>
       <c:bar3DChart>
@@ -8300,8 +8368,529 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="4"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>COPY API</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.3751494268554252E-3"/>
+                  <c:y val="1.5937857772636867E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-3FC2-40C7-8307-DB305FEC6AD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>(gaussian3!$A$1,gaussian3!$A$11,gaussian3!$A$21,gaussian3!$A$31,gaussian3!$A$41)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>traditional Allocation</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OPT traditional Allocation</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ScatterAlloc</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Zero-Copy</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Unified Memory</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(gaussian1024!$E$9,gaussian1024!$E$19,gaussian1024!$E$29,gaussian1024!$E$39,gaussian1024!$E$49)</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0796199003459837</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99923382149141415</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-4090-4208-93DC-0834A68FB2CB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>SYNC API</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>(gaussian3!$A$1,gaussian3!$A$11,gaussian3!$A$21,gaussian3!$A$31,gaussian3!$A$41)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>traditional Allocation</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OPT traditional Allocation</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ScatterAlloc</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Zero-Copy</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Unified Memory</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(gaussian1024!$F$7,gaussian1024!$F$17,gaussian1024!$F$27,gaussian1024!$F$37,gaussian1024!$F$47)</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.49685522645290497</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.52853861533333302</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.59037115000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.55035044</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0994194107142801</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5A59-4191-B28B-1F90070C00D9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>TOTAL EXEC</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>(gaussian3!$A$1,gaussian3!$A$11,gaussian3!$A$21,gaussian3!$A$31,gaussian3!$A$41)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>traditional Allocation</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OPT traditional Allocation</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ScatterAlloc</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Zero-Copy</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Unified Memory</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(gaussian1024!$K$9,gaussian1024!$K$19,gaussian1024!$K$29,gaussian1024!$K$39,gaussian1024!$K$49)</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0146750792693375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2300317818639621</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0178573065986021</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8894207030865107</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5A59-4191-B28B-1F90070C00D9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>KERNEL LAUNCH API</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>(gaussian3!$A$1,gaussian3!$A$11,gaussian3!$A$21,gaussian3!$A$31,gaussian3!$A$41)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>traditional Allocation</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OPT traditional Allocation</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ScatterAlloc</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Zero-Copy</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Unified Memory</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(gaussian1024!$C$9,gaussian1024!$C$19,gaussian1024!$C$29,gaussian1024!$C$39,gaussian1024!$C$49)</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0123884174964863</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.89595804876494023</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1191156754814064</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0118502837174415</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-D69F-44C6-9345-B374360E1564}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="1"/>
-          <c:order val="0"/>
+          <c:order val="4"/>
           <c:tx>
             <c:v>AllocAPI</c:v>
           </c:tx>
@@ -8421,507 +9010,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-5A59-4191-B28B-1F90070C00D9}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>COPY API</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-            <a:sp3d/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="bg1"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="es-ES"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>(gaussian3!$A$1,gaussian3!$A$11,gaussian3!$A$21,gaussian3!$A$31,gaussian3!$A$41)</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>traditional Allocation</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>OPT traditional Allocation</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>ScatterAlloc</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Zero-Copy</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Unified Memory</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>(gaussian1024!$E$9,gaussian1024!$E$19,gaussian1024!$E$29,gaussian1024!$E$39,gaussian1024!$E$49)</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0796199003459837</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.99923382149141415</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-4090-4208-93DC-0834A68FB2CB}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>SYNC API</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-            <a:sp3d/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="bg1"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="es-ES"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>(gaussian3!$A$1,gaussian3!$A$11,gaussian3!$A$21,gaussian3!$A$31,gaussian3!$A$41)</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>traditional Allocation</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>OPT traditional Allocation</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>ScatterAlloc</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Zero-Copy</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Unified Memory</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>(gaussian1024!$F$7,gaussian1024!$F$17,gaussian1024!$F$27,gaussian1024!$F$37,gaussian1024!$F$47)</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0.49685522645290497</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.52853861533333302</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.59037115000000007</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.55035044</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.0994194107142801</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-5A59-4191-B28B-1F90070C00D9}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>TOTAL EXEC</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-            <a:sp3d/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="bg1"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="es-ES"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>(gaussian3!$A$1,gaussian3!$A$11,gaussian3!$A$21,gaussian3!$A$31,gaussian3!$A$41)</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>traditional Allocation</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>OPT traditional Allocation</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>ScatterAlloc</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Zero-Copy</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Unified Memory</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>(gaussian1024!$K$9,gaussian1024!$K$19,gaussian1024!$K$29,gaussian1024!$K$39,gaussian1024!$K$49)</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0146750792693375</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.2300317818639621</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.0178573065986021</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.8894207030865107</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5A59-4191-B28B-1F90070C00D9}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:v>KERNEL LAUNCH API</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-            <a:sp3d/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="es-ES"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>(gaussian3!$A$1,gaussian3!$A$11,gaussian3!$A$21,gaussian3!$A$31,gaussian3!$A$41)</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>traditional Allocation</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>OPT traditional Allocation</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>ScatterAlloc</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Zero-Copy</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Unified Memory</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>(gaussian1024!$C$9,gaussian1024!$C$19,gaussian1024!$C$29,gaussian1024!$C$39,gaussian1024!$C$49)</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0123884174964863</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.89595804876494023</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.1191156754814064</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0118502837174415</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-D69F-44C6-9345-B374360E1564}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -9037,8 +9125,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="9.9884094555552569E-2"/>
-              <c:y val="0.3527248609864273"/>
+              <c:x val="4.7928992413405896E-2"/>
+              <c:y val="0.43985803251002736"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -9243,9 +9331,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.7206391626089008E-2"/>
-          <c:y val="2.2770647303387497E-2"/>
-          <c:w val="0.74041050325388946"/>
+          <c:x val="0.11705770208439248"/>
+          <c:y val="2.0687335958005249E-2"/>
+          <c:w val="0.63686479692707454"/>
           <c:h val="0.81955410382548477"/>
         </c:manualLayout>
       </c:layout>
@@ -9412,6 +9500,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -9519,8 +9608,141 @@
           </c:extLst>
         </c:ser>
         <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>gaussian1024!$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>kernels: Fan2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>(gaussian3!$A$1,gaussian3!$A$11,gaussian3!$A$21,gaussian3!$A$31,gaussian3!$A$41)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>traditional Allocation</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>OPT traditional Allocation</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ScatterAlloc</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Zero-Copy</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Unified Memory</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(gaussian1024!$J$9,gaussian1024!$J$19,gaussian1024!$J$29,gaussian1024!$J$39,gaussian1024!$J$49)</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.082825531352086</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.183230063978074</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.113471612482966</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0646954757044798</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5A59-4191-B28B-1F90070C00D9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="3"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>gaussian1024!$I$4</c:f>
@@ -9648,139 +9870,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-5A59-4191-B28B-1F90070C00D9}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>gaussian1024!$J$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>kernels: Fan2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-            <a:sp3d/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="bg1"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="es-ES"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>(gaussian3!$A$1,gaussian3!$A$11,gaussian3!$A$21,gaussian3!$A$31,gaussian3!$A$41)</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>traditional Allocation</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>OPT traditional Allocation</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>ScatterAlloc</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Zero-Copy</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Unified Memory</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>(gaussian1024!$J$9,gaussian1024!$J$19,gaussian1024!$J$29,gaussian1024!$J$39,gaussian1024!$J$49)</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.082825531352086</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.183230063978074</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.113471612482966</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.0646954757044798</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5A59-4191-B28B-1F90070C00D9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -9896,8 +9985,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="5.1493624421641675E-2"/>
-              <c:y val="0.33983517519398143"/>
+              <c:x val="3.1765378749364512E-2"/>
+              <c:y val="0.38005048905777217"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -10102,9 +10191,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.7206391626089008E-2"/>
+          <c:x val="0.10304159780485078"/>
           <c:y val="2.2770647303387497E-2"/>
-          <c:w val="0.74041050325388946"/>
+          <c:w val="0.67127637606551027"/>
           <c:h val="0.81955410382548477"/>
         </c:manualLayout>
       </c:layout>
@@ -10505,6 +10594,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -10861,8 +10951,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="5.3353037246438952E-2"/>
-              <c:y val="0.3260972629830704"/>
+              <c:x val="3.5669086211767682E-2"/>
+              <c:y val="0.40893382542040713"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -11023,7 +11113,7 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:view3D>
-      <c:rotX val="40"/>
+      <c:rotX val="50"/>
       <c:rotY val="20"/>
       <c:rAngAx val="0"/>
       <c:perspective val="0"/>
@@ -11067,10 +11157,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.7206391626089008E-2"/>
-          <c:y val="2.2770647303387497E-2"/>
-          <c:w val="0.74041050325388946"/>
-          <c:h val="0.81955410382548477"/>
+          <c:x val="0.13500574807486879"/>
+          <c:y val="2.7486424529393361E-2"/>
+          <c:w val="0.61531022878564534"/>
+          <c:h val="0.68457964418291395"/>
         </c:manualLayout>
       </c:layout>
       <c:bar3DChart>
@@ -11236,6 +11326,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -11368,6 +11459,27 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.3804439925436371E-3"/>
+                  <c:y val="9.0051762036446152E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-B2D6-4795-8646-078D9DF7C988}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
@@ -11634,6 +11746,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -11852,8 +11965,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="8.1364952057611045E-2"/>
-              <c:y val="0.38727210981255156"/>
+              <c:x val="6.1893413631690562E-2"/>
+              <c:y val="0.36343337652865892"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -11952,7 +12065,9 @@
         <c:crosses val="autoZero"/>
       </c:serAx>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:sysClr val="windowText" lastClr="000000"/>
+        </a:solidFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -11966,9 +12081,7 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="E7E6E6">
-        <a:lumMod val="50000"/>
-      </a:srgbClr>
+      <a:sysClr val="windowText" lastClr="000000"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -12060,10 +12173,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.7206391626089008E-2"/>
+          <c:x val="0.10348455710458979"/>
           <c:y val="2.2770647303387497E-2"/>
-          <c:w val="0.74041050325388946"/>
-          <c:h val="0.81955410382548477"/>
+          <c:w val="0.6736874102580882"/>
+          <c:h val="0.82402549735150754"/>
         </c:manualLayout>
       </c:layout>
       <c:bar3DChart>
@@ -12213,6 +12326,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -12989,8 +13103,8 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:view3D>
-      <c:rotX val="40"/>
-      <c:rotY val="20"/>
+      <c:rotX val="70"/>
+      <c:rotY val="30"/>
       <c:rAngAx val="0"/>
       <c:perspective val="0"/>
     </c:view3D>
@@ -13033,10 +13147,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.7206391626089008E-2"/>
-          <c:y val="2.2770647303387497E-2"/>
-          <c:w val="0.81343380178256575"/>
-          <c:h val="0.81955410382548477"/>
+          <c:x val="0.12867423600519687"/>
+          <c:y val="1.9103825482916389E-2"/>
+          <c:w val="0.611421371076174"/>
+          <c:h val="0.68929688641496756"/>
         </c:manualLayout>
       </c:layout>
       <c:bar3DChart>
@@ -13467,6 +13581,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -13981,7 +14096,7 @@
     <c:autoTitleDeleted val="1"/>
     <c:view3D>
       <c:rotX val="40"/>
-      <c:rotY val="30"/>
+      <c:rotY val="20"/>
       <c:rAngAx val="0"/>
       <c:perspective val="0"/>
     </c:view3D>
@@ -14024,9 +14139,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.7206391626089008E-2"/>
+          <c:x val="0.12210517790342745"/>
           <c:y val="2.2770647303387497E-2"/>
-          <c:w val="0.74041050325388946"/>
+          <c:w val="0.64553297991043179"/>
           <c:h val="0.81955410382548477"/>
         </c:manualLayout>
       </c:layout>
@@ -14177,6 +14292,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -14301,6 +14417,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -14649,8 +14766,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="4.2015201559950657E-2"/>
-              <c:y val="0.26484928595213125"/>
+              <c:x val="2.9677314579449811E-2"/>
+              <c:y val="0.37223408340643815"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -27831,15 +27948,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>186691</xdr:colOff>
+      <xdr:colOff>186690</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>120557</xdr:rowOff>
+      <xdr:rowOff>130081</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>176893</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>600390</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:rowOff>76448</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -27869,15 +27986,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>124867</xdr:colOff>
+      <xdr:colOff>134391</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>179983</xdr:rowOff>
+      <xdr:rowOff>170458</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>588818</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>34636</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>548091</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>78206</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -27912,15 +28029,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>179763</xdr:colOff>
+      <xdr:colOff>174048</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>346</xdr:rowOff>
+      <xdr:rowOff>345</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>311727</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>587748</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>69273</xdr:rowOff>
+      <xdr:rowOff>208390</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -27952,13 +28069,13 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>169372</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>136639</xdr:rowOff>
+      <xdr:rowOff>98193</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>259773</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>69272</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>583072</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>136866</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -28031,15 +28148,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>382904</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>169471</xdr:rowOff>
+      <xdr:colOff>592727</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>169273</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>17318</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>326070</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>21450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -28076,13 +28193,13 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>210498</xdr:rowOff>
+      <xdr:rowOff>206687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
+      <xdr:colOff>497864</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>220862</xdr:rowOff>
+      <xdr:rowOff>139546</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -28111,16 +28228,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>501438</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>104913</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>7792</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>162756</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>103909</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>421492</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>24437</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -28155,15 +28272,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>359352</xdr:colOff>
+      <xdr:colOff>359351</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>19426</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>138546</xdr:rowOff>
+      <xdr:colOff>166914</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>137070</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -28193,15 +28310,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>418608</xdr:colOff>
+      <xdr:colOff>418607</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>212348</xdr:rowOff>
+      <xdr:rowOff>212347</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>606135</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>-1</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>226170</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>74028</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -28236,15 +28353,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>411045</xdr:colOff>
+      <xdr:colOff>407235</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>203228</xdr:rowOff>
+      <xdr:rowOff>210847</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>465685</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>214799</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>139896</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -28274,15 +28391,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>472786</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>36022</xdr:rowOff>
+      <xdr:colOff>368877</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>161059</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>176441</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>20835</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -32508,7 +32625,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+      <selection activeCell="AB42" sqref="AB42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33903,7 +34020,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="Y43" sqref="Y43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35294,8 +35411,8 @@
   </sheetPr>
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:K9"/>
+    <sheetView topLeftCell="B12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y45" sqref="Y45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36686,7 +36803,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+      <selection activeCell="AB43" sqref="AB43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -38064,8 +38181,8 @@
   </sheetPr>
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AB24" sqref="AB24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39676,7 +39793,7 @@
   <dimension ref="A1:M49"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42237,14 +42354,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="b02756e4-a949-43a2-8886-57b0f09f47fd" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005AC4E0CDA633FD45AD3FBF7B00AF232F" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a4f38346409b1a654ca91995c1973336">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b02756e4-a949-43a2-8886-57b0f09f47fd" xmlns:ns4="ad9e9aeb-79f9-4415-8f12-09127192173b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6d39c616c00b869b4c90ed30090611d1" ns3:_="" ns4:_="">
     <xsd:import namespace="b02756e4-a949-43a2-8886-57b0f09f47fd"/>
@@ -42477,7 +42586,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -42486,24 +42595,15 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD9C89B2-1188-4913-8FD6-997CC58F05FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="b02756e4-a949-43a2-8886-57b0f09f47fd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ad9e9aeb-79f9-4415-8f12-09127192173b"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="b02756e4-a949-43a2-8886-57b0f09f47fd" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55CF9CEB-0A99-453B-AB49-7D58F426A4CF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -42522,10 +42622,27 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33DF58D7-67E4-457B-B2EF-D09ED4B2795A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD9C89B2-1188-4913-8FD6-997CC58F05FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="b02756e4-a949-43a2-8886-57b0f09f47fd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ad9e9aeb-79f9-4415-8f12-09127192173b"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>